<commit_message>
database credinals change new 1
</commit_message>
<xml_diff>
--- a/download/sample-csv-products.xlsx
+++ b/download/sample-csv-products.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Downloads\new20\download\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\stock_tracking\stock_tracking\download\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D048D79D-D7CB-4895-A7FB-33DB0297783E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E57E1F28-6974-4454-83D2-C32A06E423AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sample-csv-products" sheetId="1" r:id="rId1"/>
@@ -586,7 +586,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1420,10 +1420,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D148"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D148"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -1452,7 +1454,7 @@
         <v>6</v>
       </c>
       <c r="D2">
-        <v>100</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -1466,7 +1468,7 @@
         <v>6</v>
       </c>
       <c r="D3">
-        <v>200</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -1480,7 +1482,7 @@
         <v>6</v>
       </c>
       <c r="D4">
-        <v>300</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -1494,7 +1496,7 @@
         <v>6</v>
       </c>
       <c r="D5">
-        <v>400</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -1508,7 +1510,7 @@
         <v>6</v>
       </c>
       <c r="D6">
-        <v>500</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -1522,7 +1524,7 @@
         <v>6</v>
       </c>
       <c r="D7">
-        <v>600</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -1536,7 +1538,7 @@
         <v>6</v>
       </c>
       <c r="D8">
-        <v>601</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -1550,7 +1552,7 @@
         <v>6</v>
       </c>
       <c r="D9">
-        <v>602</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -1564,7 +1566,7 @@
         <v>6</v>
       </c>
       <c r="D10">
-        <v>603</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -1578,7 +1580,7 @@
         <v>6</v>
       </c>
       <c r="D11">
-        <v>604</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -1592,7 +1594,7 @@
         <v>6</v>
       </c>
       <c r="D12">
-        <v>605</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -1606,7 +1608,7 @@
         <v>6</v>
       </c>
       <c r="D13">
-        <v>606</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -1620,7 +1622,7 @@
         <v>6</v>
       </c>
       <c r="D14">
-        <v>607</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -1634,7 +1636,7 @@
         <v>6</v>
       </c>
       <c r="D15">
-        <v>608</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -1648,7 +1650,7 @@
         <v>6</v>
       </c>
       <c r="D16">
-        <v>609</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -1662,7 +1664,7 @@
         <v>6</v>
       </c>
       <c r="D17">
-        <v>610</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -1676,7 +1678,7 @@
         <v>6</v>
       </c>
       <c r="D18">
-        <v>611</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -1690,7 +1692,7 @@
         <v>6</v>
       </c>
       <c r="D19">
-        <v>612</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -1704,7 +1706,7 @@
         <v>41</v>
       </c>
       <c r="D20">
-        <v>613</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -1718,7 +1720,7 @@
         <v>41</v>
       </c>
       <c r="D21">
-        <v>614</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -1732,7 +1734,7 @@
         <v>41</v>
       </c>
       <c r="D22">
-        <v>615</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -1746,7 +1748,7 @@
         <v>41</v>
       </c>
       <c r="D23">
-        <v>616</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -1760,7 +1762,7 @@
         <v>41</v>
       </c>
       <c r="D24">
-        <v>617</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -1774,7 +1776,7 @@
         <v>47</v>
       </c>
       <c r="D25">
-        <v>618</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -1788,7 +1790,7 @@
         <v>47</v>
       </c>
       <c r="D26">
-        <v>619</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -1802,7 +1804,7 @@
         <v>47</v>
       </c>
       <c r="D27">
-        <v>620</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -1816,7 +1818,7 @@
         <v>47</v>
       </c>
       <c r="D28">
-        <v>621</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -1830,7 +1832,7 @@
         <v>47</v>
       </c>
       <c r="D29">
-        <v>622</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -1844,7 +1846,7 @@
         <v>47</v>
       </c>
       <c r="D30">
-        <v>623</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -1858,7 +1860,7 @@
         <v>47</v>
       </c>
       <c r="D31">
-        <v>624</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -1872,7 +1874,7 @@
         <v>47</v>
       </c>
       <c r="D32">
-        <v>625</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -1886,7 +1888,7 @@
         <v>47</v>
       </c>
       <c r="D33">
-        <v>626</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -1900,7 +1902,7 @@
         <v>58</v>
       </c>
       <c r="D34">
-        <v>627</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -1914,7 +1916,7 @@
         <v>58</v>
       </c>
       <c r="D35">
-        <v>628</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -1928,7 +1930,7 @@
         <v>58</v>
       </c>
       <c r="D36">
-        <v>629</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
@@ -1942,7 +1944,7 @@
         <v>58</v>
       </c>
       <c r="D37">
-        <v>630</v>
+        <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
@@ -1956,7 +1958,7 @@
         <v>58</v>
       </c>
       <c r="D38">
-        <v>631</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
@@ -1970,7 +1972,7 @@
         <v>58</v>
       </c>
       <c r="D39">
-        <v>632</v>
+        <v>5</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
@@ -1984,7 +1986,7 @@
         <v>58</v>
       </c>
       <c r="D40">
-        <v>633</v>
+        <v>5</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
@@ -1998,7 +2000,7 @@
         <v>58</v>
       </c>
       <c r="D41">
-        <v>634</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
@@ -2012,7 +2014,7 @@
         <v>58</v>
       </c>
       <c r="D42">
-        <v>635</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
@@ -2026,7 +2028,7 @@
         <v>58</v>
       </c>
       <c r="D43">
-        <v>636</v>
+        <v>5</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
@@ -2040,7 +2042,7 @@
         <v>58</v>
       </c>
       <c r="D44">
-        <v>637</v>
+        <v>5</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
@@ -2054,7 +2056,7 @@
         <v>58</v>
       </c>
       <c r="D45">
-        <v>638</v>
+        <v>5</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
@@ -2068,7 +2070,7 @@
         <v>58</v>
       </c>
       <c r="D46">
-        <v>639</v>
+        <v>5</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
@@ -2082,7 +2084,7 @@
         <v>58</v>
       </c>
       <c r="D47">
-        <v>640</v>
+        <v>5</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
@@ -2096,7 +2098,7 @@
         <v>74</v>
       </c>
       <c r="D48">
-        <v>641</v>
+        <v>5</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
@@ -2110,7 +2112,7 @@
         <v>76</v>
       </c>
       <c r="D49">
-        <v>642</v>
+        <v>5</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
@@ -2124,7 +2126,7 @@
         <v>76</v>
       </c>
       <c r="D50">
-        <v>643</v>
+        <v>5</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
@@ -2138,7 +2140,7 @@
         <v>76</v>
       </c>
       <c r="D51">
-        <v>644</v>
+        <v>5</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
@@ -2152,7 +2154,7 @@
         <v>76</v>
       </c>
       <c r="D52">
-        <v>645</v>
+        <v>5</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
@@ -2166,7 +2168,7 @@
         <v>76</v>
       </c>
       <c r="D53">
-        <v>646</v>
+        <v>5</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
@@ -2180,7 +2182,7 @@
         <v>76</v>
       </c>
       <c r="D54">
-        <v>647</v>
+        <v>5</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
@@ -2194,7 +2196,7 @@
         <v>83</v>
       </c>
       <c r="D55">
-        <v>648</v>
+        <v>5</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
@@ -2208,7 +2210,7 @@
         <v>83</v>
       </c>
       <c r="D56">
-        <v>649</v>
+        <v>5</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
@@ -2222,7 +2224,7 @@
         <v>83</v>
       </c>
       <c r="D57">
-        <v>650</v>
+        <v>5</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
@@ -2236,7 +2238,7 @@
         <v>83</v>
       </c>
       <c r="D58">
-        <v>651</v>
+        <v>5</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
@@ -2250,7 +2252,7 @@
         <v>83</v>
       </c>
       <c r="D59">
-        <v>652</v>
+        <v>5</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
@@ -2264,7 +2266,7 @@
         <v>83</v>
       </c>
       <c r="D60">
-        <v>653</v>
+        <v>5</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
@@ -2278,7 +2280,7 @@
         <v>83</v>
       </c>
       <c r="D61">
-        <v>654</v>
+        <v>5</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
@@ -2292,7 +2294,7 @@
         <v>83</v>
       </c>
       <c r="D62">
-        <v>655</v>
+        <v>5</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
@@ -2306,7 +2308,7 @@
         <v>83</v>
       </c>
       <c r="D63">
-        <v>656</v>
+        <v>5</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
@@ -2320,7 +2322,7 @@
         <v>83</v>
       </c>
       <c r="D64">
-        <v>657</v>
+        <v>5</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
@@ -2334,7 +2336,7 @@
         <v>83</v>
       </c>
       <c r="D65">
-        <v>658</v>
+        <v>5</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
@@ -2348,7 +2350,7 @@
         <v>83</v>
       </c>
       <c r="D66">
-        <v>659</v>
+        <v>5</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
@@ -2362,7 +2364,7 @@
         <v>83</v>
       </c>
       <c r="D67">
-        <v>660</v>
+        <v>5</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
@@ -2376,7 +2378,7 @@
         <v>97</v>
       </c>
       <c r="D68">
-        <v>661</v>
+        <v>5</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
@@ -2390,7 +2392,7 @@
         <v>97</v>
       </c>
       <c r="D69">
-        <v>662</v>
+        <v>5</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
@@ -2404,7 +2406,7 @@
         <v>97</v>
       </c>
       <c r="D70">
-        <v>663</v>
+        <v>5</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
@@ -2418,7 +2420,7 @@
         <v>97</v>
       </c>
       <c r="D71">
-        <v>664</v>
+        <v>5</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
@@ -2432,7 +2434,7 @@
         <v>97</v>
       </c>
       <c r="D72">
-        <v>665</v>
+        <v>5</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
@@ -2446,7 +2448,7 @@
         <v>97</v>
       </c>
       <c r="D73">
-        <v>666</v>
+        <v>5</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
@@ -2460,7 +2462,7 @@
         <v>97</v>
       </c>
       <c r="D74">
-        <v>667</v>
+        <v>5</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
@@ -2474,7 +2476,7 @@
         <v>97</v>
       </c>
       <c r="D75">
-        <v>668</v>
+        <v>5</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
@@ -2488,7 +2490,7 @@
         <v>97</v>
       </c>
       <c r="D76">
-        <v>669</v>
+        <v>5</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
@@ -2502,7 +2504,7 @@
         <v>97</v>
       </c>
       <c r="D77">
-        <v>670</v>
+        <v>5</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
@@ -2516,7 +2518,7 @@
         <v>97</v>
       </c>
       <c r="D78">
-        <v>671</v>
+        <v>5</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
@@ -2530,7 +2532,7 @@
         <v>97</v>
       </c>
       <c r="D79">
-        <v>672</v>
+        <v>5</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
@@ -2544,7 +2546,7 @@
         <v>97</v>
       </c>
       <c r="D80">
-        <v>673</v>
+        <v>5</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
@@ -2558,7 +2560,7 @@
         <v>97</v>
       </c>
       <c r="D81">
-        <v>674</v>
+        <v>5</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
@@ -2572,7 +2574,7 @@
         <v>97</v>
       </c>
       <c r="D82">
-        <v>675</v>
+        <v>5</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
@@ -2586,7 +2588,7 @@
         <v>97</v>
       </c>
       <c r="D83">
-        <v>676</v>
+        <v>5</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
@@ -2600,7 +2602,7 @@
         <v>97</v>
       </c>
       <c r="D84">
-        <v>677</v>
+        <v>5</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
@@ -2614,7 +2616,7 @@
         <v>97</v>
       </c>
       <c r="D85">
-        <v>678</v>
+        <v>5</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
@@ -2628,7 +2630,7 @@
         <v>116</v>
       </c>
       <c r="D86">
-        <v>679</v>
+        <v>5</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
@@ -2642,7 +2644,7 @@
         <v>116</v>
       </c>
       <c r="D87">
-        <v>680</v>
+        <v>5</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
@@ -2656,7 +2658,7 @@
         <v>116</v>
       </c>
       <c r="D88">
-        <v>681</v>
+        <v>5</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
@@ -2670,7 +2672,7 @@
         <v>116</v>
       </c>
       <c r="D89">
-        <v>682</v>
+        <v>5</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
@@ -2684,7 +2686,7 @@
         <v>116</v>
       </c>
       <c r="D90">
-        <v>683</v>
+        <v>5</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
@@ -2698,7 +2700,7 @@
         <v>116</v>
       </c>
       <c r="D91">
-        <v>684</v>
+        <v>5</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
@@ -2712,7 +2714,7 @@
         <v>116</v>
       </c>
       <c r="D92">
-        <v>685</v>
+        <v>5</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
@@ -2726,7 +2728,7 @@
         <v>116</v>
       </c>
       <c r="D93">
-        <v>686</v>
+        <v>5</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
@@ -2740,7 +2742,7 @@
         <v>116</v>
       </c>
       <c r="D94">
-        <v>687</v>
+        <v>5</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
@@ -2754,7 +2756,7 @@
         <v>116</v>
       </c>
       <c r="D95">
-        <v>688</v>
+        <v>5</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
@@ -2768,7 +2770,7 @@
         <v>116</v>
       </c>
       <c r="D96">
-        <v>689</v>
+        <v>5</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
@@ -2782,7 +2784,7 @@
         <v>116</v>
       </c>
       <c r="D97">
-        <v>690</v>
+        <v>5</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
@@ -2796,7 +2798,7 @@
         <v>116</v>
       </c>
       <c r="D98">
-        <v>691</v>
+        <v>5</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
@@ -2810,7 +2812,7 @@
         <v>129</v>
       </c>
       <c r="D99">
-        <v>692</v>
+        <v>5</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
@@ -2824,7 +2826,7 @@
         <v>129</v>
       </c>
       <c r="D100">
-        <v>693</v>
+        <v>5</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
@@ -2838,7 +2840,7 @@
         <v>129</v>
       </c>
       <c r="D101">
-        <v>694</v>
+        <v>5</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
@@ -2852,7 +2854,7 @@
         <v>129</v>
       </c>
       <c r="D102">
-        <v>695</v>
+        <v>5</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
@@ -2866,7 +2868,7 @@
         <v>134</v>
       </c>
       <c r="D103">
-        <v>696</v>
+        <v>5</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
@@ -2880,7 +2882,7 @@
         <v>134</v>
       </c>
       <c r="D104">
-        <v>697</v>
+        <v>5</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
@@ -2894,7 +2896,7 @@
         <v>134</v>
       </c>
       <c r="D105">
-        <v>698</v>
+        <v>5</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
@@ -2908,7 +2910,7 @@
         <v>134</v>
       </c>
       <c r="D106">
-        <v>699</v>
+        <v>5</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
@@ -2922,7 +2924,7 @@
         <v>134</v>
       </c>
       <c r="D107">
-        <v>700</v>
+        <v>5</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
@@ -2936,7 +2938,7 @@
         <v>134</v>
       </c>
       <c r="D108">
-        <v>701</v>
+        <v>5</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
@@ -2950,7 +2952,7 @@
         <v>134</v>
       </c>
       <c r="D109">
-        <v>702</v>
+        <v>5</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
@@ -2964,7 +2966,7 @@
         <v>134</v>
       </c>
       <c r="D110">
-        <v>703</v>
+        <v>5</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
@@ -2978,7 +2980,7 @@
         <v>134</v>
       </c>
       <c r="D111">
-        <v>704</v>
+        <v>5</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
@@ -2992,7 +2994,7 @@
         <v>134</v>
       </c>
       <c r="D112">
-        <v>705</v>
+        <v>5</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
@@ -3006,7 +3008,7 @@
         <v>134</v>
       </c>
       <c r="D113">
-        <v>706</v>
+        <v>5</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
@@ -3020,7 +3022,7 @@
         <v>134</v>
       </c>
       <c r="D114">
-        <v>707</v>
+        <v>5</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
@@ -3034,7 +3036,7 @@
         <v>134</v>
       </c>
       <c r="D115">
-        <v>708</v>
+        <v>5</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
@@ -3048,7 +3050,7 @@
         <v>134</v>
       </c>
       <c r="D116">
-        <v>709</v>
+        <v>5</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
@@ -3062,7 +3064,7 @@
         <v>134</v>
       </c>
       <c r="D117">
-        <v>710</v>
+        <v>5</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
@@ -3076,7 +3078,7 @@
         <v>134</v>
       </c>
       <c r="D118">
-        <v>711</v>
+        <v>5</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
@@ -3090,7 +3092,7 @@
         <v>134</v>
       </c>
       <c r="D119">
-        <v>712</v>
+        <v>5</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
@@ -3104,7 +3106,7 @@
         <v>134</v>
       </c>
       <c r="D120">
-        <v>713</v>
+        <v>5</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
@@ -3118,7 +3120,7 @@
         <v>153</v>
       </c>
       <c r="D121">
-        <v>714</v>
+        <v>5</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
@@ -3132,7 +3134,7 @@
         <v>153</v>
       </c>
       <c r="D122">
-        <v>715</v>
+        <v>5</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
@@ -3146,7 +3148,7 @@
         <v>153</v>
       </c>
       <c r="D123">
-        <v>716</v>
+        <v>5</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
@@ -3160,7 +3162,7 @@
         <v>153</v>
       </c>
       <c r="D124">
-        <v>717</v>
+        <v>5</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
@@ -3174,7 +3176,7 @@
         <v>153</v>
       </c>
       <c r="D125">
-        <v>718</v>
+        <v>5</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
@@ -3188,7 +3190,7 @@
         <v>153</v>
       </c>
       <c r="D126">
-        <v>719</v>
+        <v>5</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
@@ -3202,7 +3204,7 @@
         <v>134</v>
       </c>
       <c r="D127">
-        <v>720</v>
+        <v>5</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
@@ -3216,7 +3218,7 @@
         <v>161</v>
       </c>
       <c r="D128">
-        <v>721</v>
+        <v>5</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
@@ -3230,7 +3232,7 @@
         <v>161</v>
       </c>
       <c r="D129">
-        <v>722</v>
+        <v>5</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
@@ -3244,7 +3246,7 @@
         <v>161</v>
       </c>
       <c r="D130">
-        <v>723</v>
+        <v>5</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
@@ -3258,7 +3260,7 @@
         <v>166</v>
       </c>
       <c r="D131">
-        <v>724</v>
+        <v>5</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
@@ -3272,7 +3274,7 @@
         <v>166</v>
       </c>
       <c r="D132">
-        <v>725</v>
+        <v>5</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
@@ -3286,7 +3288,7 @@
         <v>166</v>
       </c>
       <c r="D133">
-        <v>726</v>
+        <v>5</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.3">
@@ -3300,7 +3302,7 @@
         <v>170</v>
       </c>
       <c r="D134">
-        <v>727</v>
+        <v>5</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.3">
@@ -3314,7 +3316,7 @@
         <v>170</v>
       </c>
       <c r="D135">
-        <v>728</v>
+        <v>5</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.3">
@@ -3328,7 +3330,7 @@
         <v>170</v>
       </c>
       <c r="D136">
-        <v>729</v>
+        <v>5</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.3">
@@ -3342,7 +3344,7 @@
         <v>174</v>
       </c>
       <c r="D137">
-        <v>730</v>
+        <v>5</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.3">
@@ -3356,7 +3358,7 @@
         <v>174</v>
       </c>
       <c r="D138">
-        <v>731</v>
+        <v>5</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.3">
@@ -3370,7 +3372,7 @@
         <v>174</v>
       </c>
       <c r="D139">
-        <v>732</v>
+        <v>5</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.3">
@@ -3384,7 +3386,7 @@
         <v>178</v>
       </c>
       <c r="D140">
-        <v>733</v>
+        <v>5</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.3">
@@ -3398,7 +3400,7 @@
         <v>178</v>
       </c>
       <c r="D141">
-        <v>734</v>
+        <v>5</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.3">
@@ -3412,7 +3414,7 @@
         <v>178</v>
       </c>
       <c r="D142">
-        <v>735</v>
+        <v>5</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.3">
@@ -3426,7 +3428,7 @@
         <v>178</v>
       </c>
       <c r="D143">
-        <v>736</v>
+        <v>5</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.3">
@@ -3440,7 +3442,7 @@
         <v>178</v>
       </c>
       <c r="D144">
-        <v>737</v>
+        <v>5</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.3">
@@ -3454,7 +3456,7 @@
         <v>178</v>
       </c>
       <c r="D145">
-        <v>738</v>
+        <v>5</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.3">
@@ -3468,7 +3470,7 @@
         <v>178</v>
       </c>
       <c r="D146">
-        <v>739</v>
+        <v>5</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.3">
@@ -3482,7 +3484,7 @@
         <v>178</v>
       </c>
       <c r="D147">
-        <v>740</v>
+        <v>5</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.3">
@@ -3496,7 +3498,7 @@
         <v>178</v>
       </c>
       <c r="D148">
-        <v>741</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>